<commit_message>
Documents update and structure
</commit_message>
<xml_diff>
--- a/Project/Phase 2/Sprint 3/Sprint Backlog.xlsx
+++ b/Project/Phase 2/Sprint 3/Sprint Backlog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ana Carolina Gadelha\IdeaProjects\ganttproject2\Project\Phase 2\Sprint 3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7F11F1B-CB21-40E8-AFB8-C09BAE71FD7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D467DE9-8C83-414E-880D-248ACC26605F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-45" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -430,7 +430,7 @@
   <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -473,11 +473,11 @@
       <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="3"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="4"/>
-      <c r="D3" s="3"/>
       <c r="E3" s="4" t="s">
         <v>7</v>
       </c>

</xml_diff>